<commit_message>
add: docProps/app.xml の復元, xl/ctrlProps/ フォルダの削除。
</commit_message>
<xml_diff>
--- a/考察/比較と対応.xlsx
+++ b/考察/比較と対応.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Study\Qiita記事\python\openpyxl-drawing\考察\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CEB9B6-E8A6-4D9A-95EF-984335F49343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFD519E-2077-4651-A537-C8D56576B129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="164">
   <si>
     <t>フォルダ・ファイル</t>
     <phoneticPr fontId="2"/>
@@ -39,13 +39,6 @@
     <t>対応</t>
     <rPh sb="0" eb="2">
       <t>タイオウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>済</t>
-    <rPh sb="0" eb="1">
-      <t>スミ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -12379,10 +12372,6 @@
     <rPh sb="6" eb="8">
       <t>フクゲン</t>
     </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>？</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -12618,12 +12607,253 @@
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>_rels/.rels</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>パッケージ全体のリレーションシップを定義する。</t>
+    <rPh sb="5" eb="7">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>テイギ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>並び順は変わっているが内容は同じ。</t>
+    <rPh sb="0" eb="1">
+      <t>ナラ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ジュン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>オナ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>なし。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>docProps/core.xml</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>docProps/app.xml</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>docProps/custom.xml</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>微妙に変わっているが、そのままで大丈夫そう。</t>
+    <rPh sb="0" eb="2">
+      <t>ビミョウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>ダイジョウブ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>作成者や作成日時などのメタデータ。</t>
+    <rPh sb="0" eb="3">
+      <t>サクセイシャ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ニチジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ユーザが設定したカスタムプロパティ。</t>
+    <rPh sb="4" eb="6">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>もともと無かった。</t>
+    <rPh sb="4" eb="5">
+      <t>ナ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ほとんどのタグが消えている。</t>
+    <rPh sb="8" eb="9">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&lt;HeadingPairs&gt; と &lt;TitlesOfParts&gt; を復元する。</t>
+    <rPh sb="34" eb="36">
+      <t>フクゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>作業</t>
+    <rPh sb="0" eb="2">
+      <t>サギョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>済</t>
+    <rPh sb="0" eb="1">
+      <t>スミ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>不要</t>
+    <rPh sb="0" eb="2">
+      <t>フヨウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>未</t>
+    <rPh sb="0" eb="1">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>シート数や文書の種類 などのプロパティ。
+&lt;HeadingPairs&gt; と &lt;TitlesOfParts&gt; は、シートの一覧情報やシート名を管理する。</t>
+    <rPh sb="60" eb="62">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>xl/comments/comment*.xml</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openpyxl により、xl/comments*.xml がここに移動される。</t>
+    <rPh sb="34" eb="36">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>restore_doc_props_app()</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>xl/ctrlProps/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ActiveX は使っていない想定なので、使われていない ctrlProps が生成された可能性がある。</t>
+    <rPh sb="9" eb="10">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ソウテイ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="45" eb="48">
+      <t>カノウセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>save_with_drawings()</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>openpyxl がこのフォルダの中身への参照を保持しないので、このフォルダも削除しておく。
+ただし、削除しなくても問題はなさそう (openpyxl が削除してなくても Excel で開けるので)。</t>
+    <rPh sb="17" eb="19">
+      <t>ナカミ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>モンダイ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>復元しない (復元するタグから除外する)。xl/ctrlProps/ フォルダを削除するので (ActiveX を使っていない想定なので)。</t>
+    <rPh sb="0" eb="2">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ジョガイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>ソウテイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12673,6 +12903,12 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -12708,14 +12944,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -12726,11 +12956,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -13023,371 +13269,470 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="40.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.625" style="3" customWidth="1"/>
     <col min="5" max="5" width="26.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="2"/>
+    <col min="6" max="6" width="9" style="7"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="49.5">
+    <row r="2" spans="1:6" ht="33">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="33">
-      <c r="C3" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>135</v>
+    <row r="3" spans="1:6" ht="66">
+      <c r="A3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="b">
-        <v>1</v>
+        <v>158</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="33">
-      <c r="C4" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2" t="b">
-        <v>1</v>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33">
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="33">
+      <c r="C7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="33">
+      <c r="C8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="33">
-      <c r="C6" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="49.5">
-      <c r="C7" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="2" t="b">
-        <v>1</v>
+      <c r="D8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="33">
-      <c r="C9" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="2" t="b">
-        <v>1</v>
+      <c r="A9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="33">
-      <c r="C10" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>99</v>
+    <row r="10" spans="1:6" ht="66">
+      <c r="A10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="2" t="b">
-        <v>1</v>
+        <v>161</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="2" t="b">
-        <v>1</v>
+      <c r="F11" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="2" t="b">
-        <v>1</v>
+      <c r="F12" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="2" t="b">
-        <v>1</v>
+      <c r="F13" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="2" t="b">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" s="2" t="b">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>116</v>
+      <c r="F16" s="7" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="2" t="b">
-        <v>1</v>
+        <v>115</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="2" t="b">
-        <v>1</v>
+      <c r="F18" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="33">
       <c r="A19" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F19" s="2" t="b">
-        <v>1</v>
+      <c r="C19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="66">
       <c r="A20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" s="2" t="b">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="49.5">
-      <c r="C21" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F21" s="2" t="b">
-        <v>1</v>
+      <c r="C21" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="33">
-      <c r="C22" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F22" s="2" t="b">
-        <v>1</v>
+      <c r="C22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="49.5">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F23" s="2" t="b">
-        <v>1</v>
+      <c r="F23" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="49.5">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="33">
+      <c r="C25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="33">
+      <c r="C26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="49.5">
+      <c r="C27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="33">
+      <c r="C28" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="49.5">
+      <c r="C29" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(F1&lt;&gt;"", F1=FALSE)</formula>
+      <formula>OR(F1="TODO", F1="未")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13407,393 +13752,393 @@
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="6" t="s">
-        <v>11</v>
+      <c r="A1" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="6" t="s">
-        <v>12</v>
+      <c r="A2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
+      <c r="A3" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
+      <c r="A4" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="6" t="s">
-        <v>15</v>
+      <c r="A5" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="6" t="s">
-        <v>16</v>
+      <c r="A6" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="6" t="s">
-        <v>17</v>
+      <c r="A7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="6" t="s">
-        <v>18</v>
+      <c r="A8" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="6" t="s">
-        <v>19</v>
+      <c r="A9" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="6" t="s">
-        <v>20</v>
+      <c r="A10" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="6" t="s">
-        <v>21</v>
+      <c r="A11" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="6" t="s">
-        <v>22</v>
+      <c r="A12" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="6" t="s">
-        <v>23</v>
+      <c r="A13" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="6" t="s">
-        <v>24</v>
+      <c r="A14" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="6" t="s">
-        <v>25</v>
+      <c r="A15" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="6" t="s">
-        <v>26</v>
+      <c r="A16" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="6" t="s">
-        <v>27</v>
+      <c r="A17" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="6" t="s">
-        <v>28</v>
+      <c r="A18" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="6" t="s">
-        <v>29</v>
+      <c r="A19" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="6" t="s">
-        <v>30</v>
+      <c r="A20" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="6" t="s">
-        <v>31</v>
+      <c r="A21" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="6" t="s">
-        <v>32</v>
+      <c r="A22" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="6" t="s">
-        <v>33</v>
+      <c r="A23" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="6" t="s">
-        <v>34</v>
+      <c r="A24" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="6" t="s">
-        <v>35</v>
+      <c r="A25" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="6" t="s">
-        <v>36</v>
+      <c r="A26" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="6" t="s">
-        <v>37</v>
+      <c r="A27" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="6" t="s">
-        <v>38</v>
+      <c r="A28" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="6" t="s">
-        <v>39</v>
+      <c r="A29" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="6" t="s">
-        <v>40</v>
+      <c r="A30" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="6" t="s">
-        <v>41</v>
+      <c r="A31" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="6" t="s">
-        <v>42</v>
+      <c r="A32" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="6" t="s">
-        <v>43</v>
+      <c r="A33" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="6" t="s">
-        <v>44</v>
+      <c r="A34" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="6" t="s">
-        <v>45</v>
+      <c r="A35" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="6" t="s">
-        <v>46</v>
+      <c r="A36" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="6" t="s">
-        <v>47</v>
+      <c r="A37" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="6" t="s">
-        <v>48</v>
+      <c r="A38" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="6" t="s">
-        <v>49</v>
+      <c r="A39" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="6" t="s">
-        <v>50</v>
+      <c r="A40" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="6" t="s">
-        <v>51</v>
+      <c r="A41" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="6" t="s">
-        <v>52</v>
+      <c r="A42" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="6" t="s">
-        <v>53</v>
+      <c r="A43" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="6" t="s">
-        <v>54</v>
+      <c r="A44" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="6" t="s">
-        <v>55</v>
+      <c r="A45" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="6" t="s">
-        <v>56</v>
+      <c r="A46" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="6" t="s">
-        <v>57</v>
+      <c r="A47" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="6" t="s">
-        <v>58</v>
+      <c r="A48" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="6" t="s">
-        <v>59</v>
+      <c r="A49" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="6" t="s">
-        <v>60</v>
+      <c r="A50" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="6" t="s">
-        <v>61</v>
+      <c r="A51" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="6" t="s">
-        <v>62</v>
+      <c r="A52" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="6" t="s">
-        <v>63</v>
+      <c r="A53" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="6" t="s">
-        <v>64</v>
+      <c r="A54" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="6" t="s">
-        <v>65</v>
+      <c r="A55" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="6" t="s">
-        <v>66</v>
+      <c r="A56" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="6" t="s">
-        <v>67</v>
+      <c r="A57" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="6" t="s">
-        <v>68</v>
+      <c r="A58" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="6" t="s">
-        <v>69</v>
+      <c r="A59" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="6" t="s">
-        <v>70</v>
+      <c r="A60" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="6" t="s">
-        <v>71</v>
+      <c r="A61" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="6" t="s">
-        <v>72</v>
+      <c r="A62" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="6" t="s">
-        <v>73</v>
+      <c r="A63" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="6" t="s">
-        <v>74</v>
+      <c r="A64" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="6" t="s">
-        <v>75</v>
+      <c r="A65" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="6" t="s">
-        <v>76</v>
+      <c r="A66" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="6" t="s">
-        <v>77</v>
+      <c r="A67" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="6" t="s">
-        <v>78</v>
+      <c r="A68" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="6" t="s">
-        <v>79</v>
+      <c r="A69" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="6" t="s">
-        <v>80</v>
+      <c r="A70" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="6" t="s">
-        <v>81</v>
+      <c r="A71" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="6" t="s">
-        <v>82</v>
+      <c r="A72" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="6" t="s">
-        <v>83</v>
+      <c r="A73" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="6" t="s">
-        <v>9</v>
+      <c r="A74" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="6" t="s">
-        <v>10</v>
+      <c r="A75" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="6" t="s">
-        <v>8</v>
+      <c r="A76" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="6" t="s">
-        <v>84</v>
+      <c r="A77" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="6" t="s">
-        <v>85</v>
+      <c r="A78" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change: sheet*.xml.rels から vml の Relationship を削除。
</commit_message>
<xml_diff>
--- a/考察/比較と対応.xlsx
+++ b/考察/比較と対応.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Study\Qiita記事\python\openpyxl-drawing\考察\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69A5927-0869-43CD-96BA-56F71BC74F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD12625F-C8C8-4984-9AB3-FD16499BC73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,13 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="185">
   <si>
     <t>フォルダ・ファイル</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>before x after</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -12176,22 +12172,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>&lt;Override PartName="/xl/comments*.xml" ...&gt; が
-&lt;Override PartName="/xl/comments/comment*.xml" ...&gt;
-になっている。</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>そのままで良い。calcChain.xml も復元しないため。</t>
-    <rPh sb="5" eb="6">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>フクゲン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>復元しない。</t>
     <rPh sb="0" eb="2">
       <t>フクゲン</t>
@@ -12259,19 +12239,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>保存前の zip から復元する。</t>
-    <rPh sb="0" eb="2">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>フクゲン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>restore_folder()</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -12364,13 +12331,6 @@
   <si>
     <t>&lt;Relationship Target="../ctrlProps/ctrlProp*.xml" ...&gt; が消えている。</t>
     <rPh sb="56" eb="57">
-      <t>キ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&lt;Relationship Target="../drawings/vmlDrawing*.vml" ...&gt; が消えている。</t>
-    <rPh sb="57" eb="58">
       <t>キ</t>
     </rPh>
     <phoneticPr fontId="2"/>
@@ -12665,13 +12625,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>openpyxl により、xl/comments*.xml がここに移動される。</t>
-    <rPh sb="34" eb="36">
-      <t>イドウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>restore_doc_props_app()</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -12724,36 +12677,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t xml:space="preserve">openpyxl がこのフォルダの中身への参照を保持しないので、このフォルダも削除しておく。
-ただし、削除しなくても問題はなさそう (openpyxl が削除してなくても Excel で開けるので)。
-</t>
-    <rPh sb="17" eb="19">
-      <t>ナカミ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ホジ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>サクジョ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>サクジョ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>モンダイ</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>サクジョ</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>ヒラ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>ActiveX は使っていない想定なので本来は不要。使われていない ctrlProps が残っていた可能性がある。</t>
     <rPh sb="9" eb="10">
       <t>ツカ</t>
@@ -12846,44 +12769,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">復元する。id は採番しなおす </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>(⇒ 要修正)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>。</t>
-    </r>
-    <rPh sb="0" eb="2">
-      <t>フクゲン</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>サイバン</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>シュウセイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>xl/metadata.xml</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -12893,35 +12778,6 @@
   </si>
   <si>
     <t>xl/vbaProject.bin</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">保存前の xml から復元する。
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>※r:id がそのままだが良いか。</t>
-    </r>
-    <rPh sb="0" eb="2">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>フクゲン</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>ヨ</t>
-    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -12935,32 +12791,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">コピーして復元している。
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>※復元しないように修正する。</t>
-    </r>
-    <rPh sb="5" eb="7">
-      <t>フクゲン</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>フクゲン</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>シュウセイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>openpyxl は sharedStrings を使わない形でブックを保存するので、復元しなくて良い。</t>
     <rPh sb="26" eb="27">
       <t>ツカ</t>
@@ -12976,62 +12806,6 @@
     </rPh>
     <rPh sb="49" eb="50">
       <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <r>
-      <t>復元しない。旧式の図形・コメントの名残なので。xl/comments*.xml は xl/comments/フォルダ以下に移動されている (新式になっている)。
-残っているものもあるが、削除した方が良さそう。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>(⇒ 削除するよう修正する)</t>
-    </r>
-    <rPh sb="0" eb="2">
-      <t>フクゲン</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>キュウシキ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ズケイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ナゴリ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>イドウ</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>シンシキ</t>
-    </rPh>
-    <rPh sb="81" eb="82">
-      <t>ノコ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>サクジョ</t>
-    </rPh>
-    <rPh sb="97" eb="98">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="107" eb="109">
-      <t>サクジョ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>シュウセイ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -13079,19 +12853,285 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t xml:space="preserve">リッチデータ、スピル配列、PowerQuery、セルのメタデータが使われていないので、復元しなくて良い。
+    <t>そのままで良い。xl/calcChain.xml も復元しないため。</t>
+    <rPh sb="5" eb="6">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>フクゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">リッチデータ、スピル配列、PowerQuery、セルのメタデータ が使われていないので、復元しなくて良い。
 </t>
     <rPh sb="10" eb="12">
       <t>ハイレツ</t>
     </rPh>
-    <rPh sb="33" eb="34">
+    <rPh sb="34" eb="35">
       <t>ツカ</t>
     </rPh>
+    <rPh sb="44" eb="46">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>before vs after</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">openpyxl がこのフォルダの中身への参照を保持しないので、このフォルダも削除しておく。
+ただし、削除しなくても問題はなさそう (openpyxl は削除しないが保存後も Excel で開けるので)。
+</t>
+    <rPh sb="17" eb="19">
+      <t>ナカミ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>モンダイ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="83" eb="85">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>保存前の zip から復元する。
+この内容を参照するのは xl/drawings/ フォルダ内のコンテンツだが、それもそのまま復元するのでリレーションの調整は不要。</t>
+    <rPh sb="0" eb="2">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>チョウセイ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>フヨウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&lt;Override PartName="/xl/diagrams/*.xml" ...&gt; が消えている。</t>
+    <rPh sb="46" eb="47">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Override PartName="/xl/comments*.xml" ...&gt; が
+&lt;Override PartName="/xl/comments/comment*.xml" ...&gt;
+になっている。
+</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">保存前の xml から復元する。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>※r:id は、sheet*.xml.rels 内の Relationship に合わせた方がよさそう。</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>ホウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>？</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>xl/comments*.xml</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>旧式の図形やコメント。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>新式の図形やコメント。</t>
+    <rPh sb="0" eb="2">
+      <t>シンシキ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ズケイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>なくなる (openpyxl により、xl/comments/comment*.xml に移動される)。</t>
+    <rPh sb="45" eb="47">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>新しく作られる (openpyxl により、xl/comments*.xml がここに移動される)。</t>
+    <rPh sb="0" eb="1">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ツク</t>
+    </rPh>
     <rPh sb="43" eb="45">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&lt;Relationship Target="../drawings/vmlDrawing*.vml" ...&gt; が一部消えている。</t>
+    <rPh sb="57" eb="59">
+      <t>イチブ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>復元しない。残っているものは削除する。旧式の図形・コメントの名残なので。
+xl/comments*.xml は xl/comments/フォルダ以下に移動されている (新式になっている)。</t>
+    <rPh sb="0" eb="2">
       <t>フクゲン</t>
     </rPh>
-    <rPh sb="49" eb="50">
-      <t>ヨ</t>
+    <rPh sb="6" eb="7">
+      <t>ノコ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>キュウシキ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ズケイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ナゴリ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>イドウ</t>
+    </rPh>
+    <rPh sb="84" eb="86">
+      <t>シンシキ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>復元する。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>id は 採番しなおす。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ファイル自体がなくなっている場合はファイルごと復元する。</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>サイバン</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ジタイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>フクゲン</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -13100,7 +13140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13163,6 +13203,14 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -13193,7 +13241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -13218,6 +13266,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13516,13 +13570,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -13541,514 +13595,564 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="33">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="66">
       <c r="A3" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>89</v>
+        <v>168</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="33">
+    <row r="7" spans="1:6" ht="49.5">
       <c r="C7" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>91</v>
+        <v>169</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="49.5">
+    <row r="8" spans="1:6" ht="33">
       <c r="C8" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>91</v>
+        <v>164</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="33">
       <c r="A9" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="33">
+      <c r="A10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="82.5">
+      <c r="A11" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="C11" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="82.5">
-      <c r="A10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="66">
       <c r="A12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>160</v>
+        <v>96</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="66">
       <c r="A13" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>161</v>
+        <v>100</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="66">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>121</v>
+        <v>172</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>163</v>
+        <v>102</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>145</v>
+      <c r="C16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="66">
-      <c r="A16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>145</v>
+    <row r="17" spans="1:6" ht="66">
+      <c r="A17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="82.5">
-      <c r="C17" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="33">
+    <row r="18" spans="1:6" ht="66">
       <c r="C18" s="3" t="s">
-        <v>119</v>
+        <v>182</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="49.5">
       <c r="C19" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>122</v>
+        <v>184</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="33">
-      <c r="A20" s="1" t="s">
-        <v>96</v>
-      </c>
+    <row r="20" spans="1:6" ht="49.5">
       <c r="C20" s="3" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="49.5">
+      <c r="A21" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="C21" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>177</v>
+        <v>94</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>113</v>
+        <v>165</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="33">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="33">
       <c r="A24" s="1" t="s">
-        <v>168</v>
+        <v>110</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>173</v>
+        <v>111</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="33">
+    <row r="25" spans="1:6" ht="49.5">
       <c r="A25" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="F25" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="33">
       <c r="A26" s="1" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>170</v>
+        <v>103</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="49.5">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="49.5">
+      <c r="A30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="33">
-      <c r="C30" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="33">
       <c r="C31" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="49.5">
+    <row r="32" spans="1:6" ht="33">
       <c r="C32" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="3:6" ht="33">
       <c r="C33" s="3" t="s">
-        <v>87</v>
+        <v>173</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="34" spans="3:6" ht="49.5">
+    <row r="34" spans="3:6" ht="33">
       <c r="C34" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" ht="49.5">
+      <c r="C35" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" ht="66">
+      <c r="C36" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -14076,392 +14180,392 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change: 復元した Relationship に合わせて drawing を作成。
</commit_message>
<xml_diff>
--- a/考察/比較と対応.xlsx
+++ b/考察/比較と対応.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Study\Qiita記事\python\openpyxl-drawing\考察\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BE746C-FF99-4D3A-992E-9DEF3F095DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2F60C0-1391-444B-A7C8-387E9A855A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12959,41 +12959,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">保存前の xml から復元する。
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>※r:id は、sheet*.xml.rels 内の Relationship に合わせた方がよさそう。</t>
-    </r>
-    <rPh sb="0" eb="2">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>マエ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>フクゲン</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ナイ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>ホウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>？</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -13046,39 +13011,14 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>復元しない。残っているものは削除する。旧式の図形・コメントの名残なので。
-xl/comments*.xml は xl/comments/フォルダ以下に移動されている (新式になっている)。</t>
+    <t>削除する。旧式の図形・コメントの名残なので。</t>
     <rPh sb="0" eb="2">
-      <t>フクゲン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ノコ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
       <t>サクジョ</t>
     </rPh>
-    <rPh sb="19" eb="21">
-      <t>キュウシキ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ズケイ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>ナゴリ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>イドウ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>シンシキ</t>
-    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>復元する。id は 採番しなおす。
+    <t>復元する。id は 採番しなおす (削除するものをしてから)。
 ファイル自体がなくなっている場合はファイルごと復元する。</t>
     <rPh sb="0" eb="2">
       <t>フクゲン</t>
@@ -13086,21 +13026,94 @@
     <rPh sb="10" eb="12">
       <t>サイバン</t>
     </rPh>
-    <rPh sb="22" eb="24">
+    <rPh sb="18" eb="20">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
       <t>ジタイ</t>
     </rPh>
+    <rPh sb="46" eb="48">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>フクゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>保存前の xml から復元する。
+※r:id は、sheet*.xml.rels 内の Relationship に合わせる。</t>
+    <rPh sb="0" eb="2">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>ア</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">復元しない。残っているものは削除する </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>(⇒これが良くないかも)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>。旧式の図形・コメントの名残なので。
+xl/comments*.xml は xl/comments/フォルダ以下に移動されている (新式になっている)。</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>フクゲン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ノコ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>サクジョ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ヨ</t>
+    </rPh>
     <rPh sb="32" eb="34">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>フクゲン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>削除する。旧式の図形・コメントの名残なので。</t>
-    <rPh sb="0" eb="2">
-      <t>サクジョ</t>
+      <t>キュウシキ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ズケイ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ナゴリ</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>イドウ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>シンシキ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -13542,10 +13555,10 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -13697,13 +13710,13 @@
     </row>
     <row r="9" spans="1:6" ht="33">
       <c r="A9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E9" s="8"/>
     </row>
@@ -13712,10 +13725,10 @@
         <v>143</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>140</v>
@@ -13854,24 +13867,24 @@
     </row>
     <row r="18" spans="1:6" ht="66">
       <c r="C18" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>159</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="49.5">
+    <row r="19" spans="1:6" ht="66">
       <c r="C19" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>159</v>
@@ -13898,14 +13911,14 @@
       <c r="C21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>174</v>
+      <c r="D21" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -13913,7 +13926,7 @@
         <v>165</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>95</v>
@@ -13989,7 +14002,7 @@
         <v>105</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:6">

</xml_diff>